<commit_message>
working on filter options
</commit_message>
<xml_diff>
--- a/Data/laserJobs.xlsx
+++ b/Data/laserJobs.xlsx
@@ -822,17 +822,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>david</t>
+          <t>pepe</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>2019-12-22</t>
+          <t>2019-12-27</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Alumina</t>
+          <t>organic</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">

</xml_diff>

<commit_message>
working on filter options2
</commit_message>
<xml_diff>
--- a/Data/laserJobs.xlsx
+++ b/Data/laserJobs.xlsx
@@ -326,7 +326,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -876,6 +876,638 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>david</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>pmma</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>david</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>pmma</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>david</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>pmma</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>david</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>pmma</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>David</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>pmma</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>david</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>sache</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2019-12-27</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
Improved text filtering. Now case-sensitive, and option and whole-word option Added config.json for the persience of the textFilter settings
</commit_message>
<xml_diff>
--- a/Data/laserJobs.xlsx
+++ b/Data/laserJobs.xlsx
@@ -326,7 +326,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -1460,13 +1460,11 @@
       <c r="A20" t="n">
         <v>19</v>
       </c>
-      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
           <t>2019-12-27</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
           <t>Cut</t>
@@ -1503,6 +1501,246 @@
         </is>
       </c>
       <c r="L20" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>david</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2020-01-02</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>pmma</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>david</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2020-01-02</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>pmma</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>sads</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2020-01-02</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Enter here useful comments for the future</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>aS</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2020-01-02</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Asa</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Cut</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>900</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>1/0</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
         <is>
           <t>Enter here useful comments for the future</t>
         </is>

</xml_diff>